<commit_message>
fixed 0 quantity error
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2934000</v>
+        <v>3368900</v>
       </c>
       <c r="C2" t="n">
         <v>2233110.891089109</v>
@@ -481,10 +481,10 @@
         <v>0.01010000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>7078.980000000002</v>
+        <v>11471.47000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>31.38622052794971</v>
+        <v>50.86129459325488</v>
       </c>
     </row>
     <row r="3">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11400</v>
+        <v>13975</v>
       </c>
       <c r="C3" t="n">
         <v>11186.23481781377</v>
@@ -503,34 +503,10 @@
         <v>494</v>
       </c>
       <c r="E3" t="n">
-        <v>105599.9999999999</v>
+        <v>1377650</v>
       </c>
       <c r="F3" t="n">
-        <v>1.910966340933766</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>ethinr</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>120006.6</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2334</v>
-      </c>
-      <c r="D4" t="n">
-        <v>21</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2471124.6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>5041.670951156812</v>
+        <v>24.93032935215346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>